<commit_message>
UNI-0001 <I> Fix bug that lets user click on the playing board (and the board updates!!)  even after game result has been decided.
</commit_message>
<xml_diff>
--- a/BugTracker.xlsx
+++ b/BugTracker.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="58">
   <si>
     <t>Type</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t>PA : PracticeArea? (UNI : Unipoles)</t>
+  </si>
+  <si>
+    <t>&lt;I&gt; Fix bug that lets user click on the playing board (and the board updates!!)  even after game result has been decided.</t>
+  </si>
+  <si>
+    <t>11/15/2013 22:37:42</t>
+  </si>
+  <si>
+    <t>Clicking anywhere on the board should not result in any update once player has won/lost.</t>
   </si>
 </sst>
 </file>
@@ -555,7 +564,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -607,7 +615,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -631,11 +639,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2097562392"/>
-        <c:axId val="2097200664"/>
+        <c:axId val="2131554552"/>
+        <c:axId val="2131579208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2097562392"/>
+        <c:axId val="2131554552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,7 +652,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097200664"/>
+        <c:crossAx val="2131579208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -652,7 +660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097200664"/>
+        <c:axId val="2131579208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.0"/>
@@ -664,7 +672,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097562392"/>
+        <c:crossAx val="2131554552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -720,7 +728,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -778,7 +785,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -835,7 +842,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -854,11 +861,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="2112467384"/>
-        <c:axId val="2112468792"/>
+        <c:axId val="2097197336"/>
+        <c:axId val="2098155272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2112467384"/>
+        <c:axId val="2097197336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -867,7 +874,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112468792"/>
+        <c:crossAx val="2098155272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -875,7 +882,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2112468792"/>
+        <c:axId val="2098155272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.0"/>
@@ -892,7 +899,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2112467384"/>
+        <c:crossAx val="2097197336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -908,7 +915,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -938,7 +944,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -987,7 +992,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -1008,11 +1013,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2110963400"/>
-        <c:axId val="2110964808"/>
+        <c:axId val="2097870680"/>
+        <c:axId val="2097261208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110963400"/>
+        <c:axId val="2097870680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1021,7 +1026,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110964808"/>
+        <c:crossAx val="2097261208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1029,7 +1034,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110964808"/>
+        <c:axId val="2097261208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1040,7 +1045,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110963400"/>
+        <c:crossAx val="2097870680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1054,7 +1059,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1084,7 +1088,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1145,7 +1148,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -1178,11 +1181,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2112461640"/>
-        <c:axId val="2112440392"/>
+        <c:axId val="2097389560"/>
+        <c:axId val="2097435832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2112461640"/>
+        <c:axId val="2097389560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1191,7 +1194,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112440392"/>
+        <c:crossAx val="2097435832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1199,7 +1202,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2112440392"/>
+        <c:axId val="2097435832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.0"/>
@@ -1211,7 +1214,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112461640"/>
+        <c:crossAx val="2097389560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1227,7 +1230,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1257,7 +1259,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1315,7 +1316,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -1339,11 +1340,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2112796680"/>
-        <c:axId val="2131490792"/>
+        <c:axId val="2097745624"/>
+        <c:axId val="2097750648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2112796680"/>
+        <c:axId val="2097745624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1352,7 +1353,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2131490792"/>
+        <c:crossAx val="2097750648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1360,7 +1361,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2131490792"/>
+        <c:axId val="2097750648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.0"/>
@@ -1372,7 +1373,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112796680"/>
+        <c:crossAx val="2097745624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1388,7 +1389,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1927,11 +1927,11 @@
       </c>
       <c r="I2" s="13" t="str">
         <f ca="1">TEXT(NOW(),"mm/dd/yyyy hh:mm:ss")</f>
-        <v>11/15/2013 22:08:36</v>
+        <v>11/15/2013 22:39:11</v>
       </c>
       <c r="J2" s="13" t="str">
         <f ca="1">TEXT(NOW(),"mm/dd/yyyy hh:mm:ss")</f>
-        <v>11/15/2013 22:08:36</v>
+        <v>11/15/2013 22:39:11</v>
       </c>
       <c r="K2" s="13"/>
     </row>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="B2" s="12">
         <f>COUNTIF(Main!A$2:A$1048576,"Bug")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="M2" s="12">
         <f>COUNTIF(Main!F$2:F$1048576,"Low")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2189,11 +2189,11 @@
       </c>
       <c r="G4" s="12">
         <f>COUNTIF(Main!D$2:D$1048576,"rhdelaro")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="12">
         <f>COUNTIF(Main!E$2:E$1048576,"rhdelaro")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
@@ -2245,7 +2245,7 @@
       </c>
       <c r="B27" s="12">
         <f>COUNTIF(Main!G$2:G$1048576,"Open")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" s="9" t="s">
         <v>36</v>
@@ -2268,7 +2268,7 @@
       </c>
       <c r="K28" s="12">
         <f>COUNTIF(Main!H$2:H$1048576,"Unresolved")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2354,7 +2354,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2406,8 +2406,37 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="E2" s="15"/>
+    <row r="2" spans="1:11" ht="42">
+      <c r="A2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="3" spans="1:11">
       <c r="I3" s="14"/>

</xml_diff>

<commit_message>
UNI-0002 <I> First big update; updated button images, logic controller, LHDataLevels, LHUIButton extended from UIButton
</commit_message>
<xml_diff>
--- a/BugTracker.xlsx
+++ b/BugTracker.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="60">
   <si>
     <t>Type</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>Clicking anywhere on the board should not result in any update once player has won/lost.</t>
+  </si>
+  <si>
+    <t>&lt;I&gt; First big update. New image for buttons, updated controller logic, updated LHDataLevels, extended UIButton to LHUIButton</t>
+  </si>
+  <si>
+    <t>11/18/2013 06:40:18</t>
   </si>
 </sst>
 </file>
@@ -621,7 +627,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -639,11 +645,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2131554552"/>
-        <c:axId val="2131579208"/>
+        <c:axId val="2127240664"/>
+        <c:axId val="2127245256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2131554552"/>
+        <c:axId val="2127240664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -652,7 +658,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2131579208"/>
+        <c:crossAx val="2127245256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -660,7 +666,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2131579208"/>
+        <c:axId val="2127245256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.0"/>
@@ -672,7 +678,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2131554552"/>
+        <c:crossAx val="2127240664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -785,7 +791,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -842,7 +848,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -861,11 +867,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="2097197336"/>
-        <c:axId val="2098155272"/>
+        <c:axId val="2127277416"/>
+        <c:axId val="2127280392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2097197336"/>
+        <c:axId val="2127277416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,7 +880,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2098155272"/>
+        <c:crossAx val="2127280392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -882,7 +888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2098155272"/>
+        <c:axId val="2127280392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.0"/>
@@ -899,7 +905,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2097197336"/>
+        <c:crossAx val="2127277416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -992,7 +998,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -1013,11 +1019,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2097870680"/>
-        <c:axId val="2097261208"/>
+        <c:axId val="2127306296"/>
+        <c:axId val="2127309240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2097870680"/>
+        <c:axId val="2127306296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1026,7 +1032,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097261208"/>
+        <c:crossAx val="2127309240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1034,7 +1040,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097261208"/>
+        <c:axId val="2127309240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1045,7 +1051,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097870680"/>
+        <c:crossAx val="2127306296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1154,7 +1160,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -1181,11 +1187,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2097389560"/>
-        <c:axId val="2097435832"/>
+        <c:axId val="2127336328"/>
+        <c:axId val="2127339336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2097389560"/>
+        <c:axId val="2127336328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1194,7 +1200,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097435832"/>
+        <c:crossAx val="2127339336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1202,7 +1208,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097435832"/>
+        <c:axId val="2127339336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.0"/>
@@ -1214,7 +1220,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097389560"/>
+        <c:crossAx val="2127336328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1316,7 +1322,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -1340,11 +1346,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2097745624"/>
-        <c:axId val="2097750648"/>
+        <c:axId val="2127366056"/>
+        <c:axId val="2127369000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2097745624"/>
+        <c:axId val="2127366056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1353,7 +1359,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097750648"/>
+        <c:crossAx val="2127369000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1361,7 +1367,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097750648"/>
+        <c:axId val="2127369000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.0"/>
@@ -1373,7 +1379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097745624"/>
+        <c:crossAx val="2127366056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1927,11 +1933,11 @@
       </c>
       <c r="I2" s="13" t="str">
         <f ca="1">TEXT(NOW(),"mm/dd/yyyy hh:mm:ss")</f>
-        <v>11/15/2013 22:39:11</v>
+        <v>11/18/2013 06:40:21</v>
       </c>
       <c r="J2" s="13" t="str">
         <f ca="1">TEXT(NOW(),"mm/dd/yyyy hh:mm:ss")</f>
-        <v>11/15/2013 22:39:11</v>
+        <v>11/18/2013 06:40:21</v>
       </c>
       <c r="K2" s="13"/>
     </row>
@@ -2142,7 +2148,7 @@
       </c>
       <c r="M2" s="12">
         <f>COUNTIF(Main!F$2:F$1048576,"Low")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2180,7 +2186,7 @@
       </c>
       <c r="B4" s="12">
         <f>COUNTIF(Main!A$2:A$1048576,"Feature")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -2189,11 +2195,11 @@
       </c>
       <c r="G4" s="12">
         <f>COUNTIF(Main!D$2:D$1048576,"rhdelaro")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" s="12">
         <f>COUNTIF(Main!E$2:E$1048576,"rhdelaro")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
@@ -2268,7 +2274,7 @@
       </c>
       <c r="K28" s="12">
         <f>COUNTIF(Main!H$2:H$1048576,"Unresolved")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2277,7 +2283,7 @@
       </c>
       <c r="B29" s="12">
         <f>COUNTIF(Main!G$2:G$1048576,"Development")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" s="10" t="s">
         <v>35</v>
@@ -2365,7 +2371,7 @@
     <col min="4" max="4" width="9.6640625" style="12" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="12" customWidth="1"/>
     <col min="6" max="6" width="10" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="17.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.6640625" style="19" customWidth="1"/>
@@ -2438,8 +2444,34 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="I3" s="14"/>
+    <row r="3" spans="1:11" ht="28">
+      <c r="A3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">

</xml_diff>

<commit_message>
Added feature tickets : UNI-0003 to UNI-0009
</commit_message>
<xml_diff>
--- a/BugTracker.xlsx
+++ b/BugTracker.xlsx
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="88">
   <si>
     <t>Type</t>
   </si>
@@ -265,6 +265,90 @@
   </si>
   <si>
     <t>11/18/2013 06:40:18</t>
+  </si>
+  <si>
+    <t>12/15/2013 07:29:50</t>
+  </si>
+  <si>
+    <t>12/15/2013 07:30:27</t>
+  </si>
+  <si>
+    <t>&lt;I&gt; Email/Feedback feature</t>
+  </si>
+  <si>
+    <t>12/15/2013 09:23:49</t>
+  </si>
+  <si>
+    <t>User button for sending email/feedback</t>
+  </si>
+  <si>
+    <t>12/15/2013 09:25:05</t>
+  </si>
+  <si>
+    <t>Feature to save/load/reset progress</t>
+  </si>
+  <si>
+    <t>&lt;I&gt; Saving/Loading/resetting progress</t>
+  </si>
+  <si>
+    <t>UNI-0005</t>
+  </si>
+  <si>
+    <t>&lt;I&gt; Tick mark for solving levels</t>
+  </si>
+  <si>
+    <t>12/15/2013 09:27:02</t>
+  </si>
+  <si>
+    <t>Display 'check' (completed) or 'star' (completed without mistake) for each of the completed levels</t>
+  </si>
+  <si>
+    <t>UNI-0006</t>
+  </si>
+  <si>
+    <t>&lt;I&gt; Achievements</t>
+  </si>
+  <si>
+    <t>12/15/2013 09:30:43</t>
+  </si>
+  <si>
+    <t>Achievements/GameCenter(?)</t>
+  </si>
+  <si>
+    <t>UNI-0007</t>
+  </si>
+  <si>
+    <t>&lt;I&gt; Enable 'Settings' button</t>
+  </si>
+  <si>
+    <t>12/15/2013 09:31:58</t>
+  </si>
+  <si>
+    <t>Setting sounds and/or brightness</t>
+  </si>
+  <si>
+    <t>UNI-0008</t>
+  </si>
+  <si>
+    <t>&lt;I&gt; Map of levels per difficulty</t>
+  </si>
+  <si>
+    <t>12/15/2013 09:34:24</t>
+  </si>
+  <si>
+    <t>Levels map with completion tick marks</t>
+  </si>
+  <si>
+    <t>UNI-0009</t>
+  </si>
+  <si>
+    <t>&lt;I&gt; Hints</t>
+  </si>
+  <si>
+    <t>12/15/2013 09:35:36</t>
+  </si>
+  <si>
+    <t>Hints (for sale?)</t>
   </si>
 </sst>
 </file>
@@ -492,7 +576,18 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -627,7 +722,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -645,11 +740,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2127240664"/>
-        <c:axId val="2127245256"/>
+        <c:axId val="2070821336"/>
+        <c:axId val="2070824840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127240664"/>
+        <c:axId val="2070821336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +753,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127245256"/>
+        <c:crossAx val="2070824840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -666,7 +761,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127245256"/>
+        <c:axId val="2070824840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.0"/>
@@ -678,7 +773,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127240664"/>
+        <c:crossAx val="2070821336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -791,7 +886,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -848,7 +943,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -867,11 +962,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="-25"/>
-        <c:axId val="2127277416"/>
-        <c:axId val="2127280392"/>
+        <c:axId val="2070865336"/>
+        <c:axId val="2070868312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127277416"/>
+        <c:axId val="2070865336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -880,7 +975,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127280392"/>
+        <c:crossAx val="2070868312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -888,7 +983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127280392"/>
+        <c:axId val="2070868312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5.0"/>
@@ -905,7 +1000,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2127277416"/>
+        <c:crossAx val="2070865336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -998,7 +1093,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -1019,11 +1114,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2127306296"/>
-        <c:axId val="2127309240"/>
+        <c:axId val="2070894120"/>
+        <c:axId val="2070897064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127306296"/>
+        <c:axId val="2070894120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,7 +1127,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127309240"/>
+        <c:crossAx val="2070897064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1040,7 +1135,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127309240"/>
+        <c:axId val="2070897064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1051,7 +1146,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127306296"/>
+        <c:crossAx val="2070894120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1154,13 +1249,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
@@ -1172,7 +1267,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1187,11 +1282,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2127336328"/>
-        <c:axId val="2127339336"/>
+        <c:axId val="2070234904"/>
+        <c:axId val="2070283448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127336328"/>
+        <c:axId val="2070234904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1200,7 +1295,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127339336"/>
+        <c:crossAx val="2070283448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1208,7 +1303,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127339336"/>
+        <c:axId val="2070283448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.0"/>
@@ -1220,7 +1315,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127336328"/>
+        <c:crossAx val="2070234904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1319,16 +1414,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.0</c:v>
@@ -1346,11 +1441,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2127366056"/>
-        <c:axId val="2127369000"/>
+        <c:axId val="2070238744"/>
+        <c:axId val="2070188280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127366056"/>
+        <c:axId val="2070238744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1359,7 +1454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127369000"/>
+        <c:crossAx val="2070188280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1367,7 +1462,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127369000"/>
+        <c:axId val="2070188280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.0"/>
@@ -1379,7 +1474,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127366056"/>
+        <c:crossAx val="2070238744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
@@ -1933,11 +2028,11 @@
       </c>
       <c r="I2" s="13" t="str">
         <f ca="1">TEXT(NOW(),"mm/dd/yyyy hh:mm:ss")</f>
-        <v>11/18/2013 06:40:21</v>
+        <v>12/15/2013 09:35:48</v>
       </c>
       <c r="J2" s="13" t="str">
         <f ca="1">TEXT(NOW(),"mm/dd/yyyy hh:mm:ss")</f>
-        <v>11/18/2013 06:40:21</v>
+        <v>12/15/2013 09:35:48</v>
       </c>
       <c r="K2" s="13"/>
     </row>
@@ -2148,7 +2243,7 @@
       </c>
       <c r="M2" s="12">
         <f>COUNTIF(Main!F$2:F$1048576,"Low")</f>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2186,7 +2281,7 @@
       </c>
       <c r="B4" s="12">
         <f>COUNTIF(Main!A$2:A$1048576,"Feature")</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -2195,11 +2290,11 @@
       </c>
       <c r="G4" s="12">
         <f>COUNTIF(Main!D$2:D$1048576,"rhdelaro")</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H4" s="12">
         <f>COUNTIF(Main!E$2:E$1048576,"rhdelaro")</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
@@ -2251,14 +2346,14 @@
       </c>
       <c r="B27" s="12">
         <f>COUNTIF(Main!G$2:G$1048576,"Open")</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J27" s="9" t="s">
         <v>36</v>
       </c>
       <c r="K27" s="12">
         <f>COUNTIF(Main!H$2:H$1048576,"Completed (Task/Feature)")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2274,7 +2369,7 @@
       </c>
       <c r="K28" s="12">
         <f>COUNTIF(Main!H$2:H$1048576,"Unresolved")</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2283,7 +2378,7 @@
       </c>
       <c r="B29" s="12">
         <f>COUNTIF(Main!G$2:G$1048576,"Development")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" s="10" t="s">
         <v>35</v>
@@ -2306,7 +2401,7 @@
       </c>
       <c r="K30" s="12">
         <f>COUNTIF(Main!H$2:H$1048576,"Fixed (Bug/Defect)")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2340,7 +2435,7 @@
       </c>
       <c r="B33" s="12">
         <f>COUNTIF(Main!G$2:G$1048576,"Closed")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2357,10 +2452,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2372,7 +2467,7 @@
     <col min="5" max="5" width="10.83203125" style="12" customWidth="1"/>
     <col min="6" max="6" width="10" style="12" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="17.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.6640625" style="19" customWidth="1"/>
   </cols>
@@ -2432,13 +2527,16 @@
         <v>30</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>56</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="K2" s="19" t="s">
         <v>57</v>
@@ -2464,23 +2562,250 @@
         <v>30</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>59</v>
       </c>
+      <c r="J3" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28">
+      <c r="A4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="42">
+      <c r="A6" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="28">
+      <c r="A9" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Blocked">
+  <conditionalFormatting sqref="G1:G1048576 H5">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2741,12 +3066,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F5">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G5">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",G1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>